<commit_message>
getting the address and present it into the view complete done
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Subject</t>
   </si>
@@ -88,16 +88,28 @@
     <t>Had to study the whole Google maps API and deal with restrictions</t>
   </si>
   <si>
-    <t xml:space="preserve">Getting the address </t>
-  </si>
-  <si>
     <t>Google maps API</t>
   </si>
   <si>
     <t>Asking user to turn on gps</t>
   </si>
   <si>
-    <t>15.5</t>
+    <t>Phone call towards RZR</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Getting the address +and present it to the view</t>
+  </si>
+  <si>
+    <t>trying to present the view with multiple lines</t>
+  </si>
+  <si>
+    <t>I have to implement a infowindow adapter but there is no priority in doing that</t>
+  </si>
+  <si>
+    <t>16.5</t>
   </si>
 </sst>
 </file>
@@ -520,7 +532,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +566,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -664,7 +676,7 @@
     </row>
     <row r="12" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5">
         <v>7</v>
@@ -677,23 +689,27 @@
     </row>
     <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
@@ -705,58 +721,68 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
     </row>
     <row r="33" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Google maps op de juiste stand, Hoofdscherm achtergrond verbeterd. Backbutton test
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Subject</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>This was a little harder than expected, Android 6.0 Marshmallow you need to implement the permissions request all by yourself. But I got it now :)</t>
+  </si>
+  <si>
+    <t>All Strings into the Strings.xml</t>
+  </si>
+  <si>
+    <t>21.5</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>button variable names and title app change</t>
   </si>
 </sst>
 </file>
@@ -538,7 +550,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,8 +583,8 @@
       <c r="B2" s="5"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="6">
-        <v>21</v>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -768,10 +780,26 @@
       </c>
     </row>
     <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>

</xml_diff>

<commit_message>
Toolbar kleur en bij elke activity
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Subject</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>button variable names and title app change</t>
+  </si>
+  <si>
+    <t>Correcting google maps zooming</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>color toolbar</t>
   </si>
 </sst>
 </file>
@@ -550,7 +562,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,10 +814,26 @@
       </c>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>

</xml_diff>

<commit_message>
proberen 9patch en drawable om te scalen maar nog niet helemaal gelukt
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Subject</t>
   </si>
@@ -52,27 +52,15 @@
     <t>Example 2</t>
   </si>
   <si>
-    <t>Had issues with scaling the background properly</t>
-  </si>
-  <si>
     <t>Layout splashscreen</t>
   </si>
   <si>
     <t>Layout toolbar</t>
   </si>
   <si>
-    <t>The correct color, icon and backbutton</t>
-  </si>
-  <si>
     <t>Layout toolbar buttons</t>
   </si>
   <si>
-    <t>I don't know how to place the buttons at the correct place(there must be a standard implementation for this)</t>
-  </si>
-  <si>
-    <t>Only issue here is I'm doubting whether I should cut the images and edit them so they fit exactly like the real RSR App, or its just more important to make the working functions</t>
-  </si>
-  <si>
     <t>Made a Github repository, Studied the files I have and the urls ive been recommanded to read. Checked some examples for android applications</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
     <t>0.5</t>
   </si>
   <si>
-    <t>Had to study the whole Google maps API and deal with restrictions</t>
-  </si>
-  <si>
     <t>Google maps API</t>
   </si>
   <si>
@@ -103,19 +88,10 @@
     <t>trying to present the view with multiple lines</t>
   </si>
   <si>
-    <t>I have to implement a infowindow adapter but there is no priority in doing that</t>
-  </si>
-  <si>
     <t>Phone call button in the google maps activity</t>
   </si>
   <si>
     <t>Asking user to turn on internet</t>
-  </si>
-  <si>
-    <t>I didnt know there was an attribute for it but I fixed it</t>
-  </si>
-  <si>
-    <t>This was a little harder than expected, Android 6.0 Marshmallow you need to implement the permissions request all by yourself. But I got it now :)</t>
   </si>
   <si>
     <t>All Strings into the Strings.xml</t>
@@ -562,7 +538,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +572,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -641,198 +617,198 @@
     </row>
     <row r="7" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5">
         <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
custom google maps window adapter alleen nog goed stylen
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Subject</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>color toolbar</t>
+  </si>
+  <si>
+    <t>can't get the button to scale right</t>
+  </si>
+  <si>
+    <t>9-patch and drawable</t>
+  </si>
+  <si>
+    <t>google maps custom infowindow</t>
+  </si>
+  <si>
+    <t>had problem with getting the correct xml layout</t>
   </si>
 </sst>
 </file>
@@ -537,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,10 +824,26 @@
       </c>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="5">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>

</xml_diff>

<commit_message>
infoscherm verbetert en poging met google maps infowindow
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>Subject</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>had problem with getting the correct xml layout</t>
+  </si>
+  <si>
+    <t>Infoscherm verbetert</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>transparent color done but still can't got the layout right</t>
   </si>
 </sst>
 </file>
@@ -549,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,10 +855,26 @@
       </c>
     </row>
     <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>

</xml_diff>

<commit_message>
drawable left en 9-patch toegepast, button scaled nu wel op mijn mobiel wanneer ik hem kantel. hoop dat hij het ook op jullie device doet
</commit_message>
<xml_diff>
--- a/Hours log.xlsx
+++ b/Hours log.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Subject</t>
   </si>
@@ -97,9 +97,6 @@
     <t>All Strings into the Strings.xml</t>
   </si>
   <si>
-    <t>21.5</t>
-  </si>
-  <si>
     <t>0.0</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>color toolbar</t>
   </si>
   <si>
-    <t>can't get the button to scale right</t>
-  </si>
-  <si>
     <t>9-patch and drawable</t>
   </si>
   <si>
@@ -137,6 +131,21 @@
   </si>
   <si>
     <t>transparent color done but still can't got the layout right</t>
+  </si>
+  <si>
+    <t>scaling the RSR Pechhulp button</t>
+  </si>
+  <si>
+    <t>still cant manage it to scale when I rotate my phone</t>
+  </si>
+  <si>
+    <t>can't get the button to scale right when I rotate</t>
+  </si>
+  <si>
+    <t>done(it works on my phone I hope it does work on your device too) solved by adding paddings</t>
+  </si>
+  <si>
+    <t>37.5</t>
   </si>
 </sst>
 </file>
@@ -558,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +602,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -801,10 +810,10 @@
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -812,10 +821,10 @@
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -823,10 +832,10 @@
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -834,32 +843,32 @@
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="5">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -867,20 +876,36 @@
     </row>
     <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5">
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-    </row>
     <row r="28" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>

</xml_diff>